<commit_message>
fix: updating to rpaframework 28.4.1 for known Get Range issue
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\koodi\testground\ally-excel-issue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Documents\Copy-Sheet-to-Sheet-Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0519F7-A17C-41BA-9595-59262A7ED599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48CB646-4EDD-41D0-852E-4EA8F7C17EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31740" yWindow="5175" windowWidth="15300" windowHeight="8745" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6660" yWindow="3885" windowWidth="20160" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -369,7 +369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
@@ -419,7 +419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAEDD6C-EAED-4558-A6DD-A3CF1F1E3810}">
   <dimension ref="B4:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>